<commit_message>
0.9, correct hybrid logic
</commit_message>
<xml_diff>
--- a/results/consolidated_test_report_0812241131.xlsx
+++ b/results/consolidated_test_report_0812241131.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rodolfocacacho/Documents/Documents/MAI/Master Thesis/Code/rag_project/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BB90216-2411-B548-94B7-B8A43517B91E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E5C255E-1A4D-AA43-81F9-249558F4A1A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-51200" yWindow="-7800" windowWidth="33060" windowHeight="28800" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-51200" yWindow="-7800" windowWidth="51200" windowHeight="28800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -515,55 +515,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="62">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFF00"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFF00"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="57">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1124,6 +1076,14 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFF00"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1424,11 +1384,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:T13"/>
   <sheetViews>
-    <sheetView zoomScale="222" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="222" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2:T13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1495,7 +1454,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>20</v>
       </c>
@@ -1557,7 +1516,7 @@
         <v>0.64704045822784817</v>
       </c>
     </row>
-    <row r="3" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>21</v>
       </c>
@@ -1619,7 +1578,7 @@
         <v>0.65927636202531636</v>
       </c>
     </row>
-    <row r="4" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -1681,7 +1640,7 @@
         <v>0.66493273670886066</v>
       </c>
     </row>
-    <row r="5" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>23</v>
       </c>
@@ -1743,7 +1702,7 @@
         <v>0.64775577721518984</v>
       </c>
     </row>
-    <row r="6" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>24</v>
       </c>
@@ -2053,7 +2012,7 @@
         <v>0.66555539240506334</v>
       </c>
     </row>
-    <row r="11" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>29</v>
       </c>
@@ -2115,7 +2074,7 @@
         <v>0.67556923797468338</v>
       </c>
     </row>
-    <row r="12" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>30</v>
       </c>
@@ -2177,7 +2136,7 @@
         <v>0.63314706075949367</v>
       </c>
     </row>
-    <row r="13" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>31</v>
       </c>
@@ -2240,18 +2199,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:T13" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <filterColumn colId="1">
-      <filters>
-        <filter val="jinaai/jina-embeddings-v3"/>
-      </filters>
-    </filterColumn>
-    <filterColumn colId="2">
-      <filters>
-        <filter val="500"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:T13" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <conditionalFormatting sqref="J2:J13">
     <cfRule type="colorScale" priority="24">
       <colorScale>
@@ -2311,11 +2259,11 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="top10" dxfId="61" priority="2" bottom="1" rank="1"/>
-    <cfRule type="top10" dxfId="60" priority="3" rank="2"/>
+    <cfRule type="top10" dxfId="55" priority="2" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="54" priority="3" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="O2:O13">
-    <cfRule type="top10" dxfId="59" priority="26" rank="2"/>
+    <cfRule type="top10" dxfId="53" priority="26" rank="2"/>
     <cfRule type="colorScale" priority="19">
       <colorScale>
         <cfvo type="min"/>
@@ -2326,7 +2274,7 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="top10" dxfId="58" priority="25" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="52" priority="25" bottom="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="P2:P13">
     <cfRule type="colorScale" priority="16">
@@ -2339,12 +2287,12 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="top10" dxfId="57" priority="17" bottom="1" rank="1"/>
-    <cfRule type="top10" dxfId="56" priority="18" rank="2"/>
+    <cfRule type="top10" dxfId="51" priority="17" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="50" priority="18" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q2:Q13">
-    <cfRule type="top10" dxfId="55" priority="14" bottom="1" rank="1"/>
-    <cfRule type="top10" dxfId="54" priority="15" rank="2"/>
+    <cfRule type="top10" dxfId="49" priority="14" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="48" priority="15" rank="2"/>
     <cfRule type="colorScale" priority="13">
       <colorScale>
         <cfvo type="min"/>
@@ -2367,12 +2315,12 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="top10" dxfId="53" priority="11" bottom="1" rank="1"/>
-    <cfRule type="top10" dxfId="52" priority="12" rank="2"/>
+    <cfRule type="top10" dxfId="47" priority="11" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="46" priority="12" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="S2:S13">
-    <cfRule type="top10" dxfId="51" priority="9" rank="2"/>
-    <cfRule type="top10" dxfId="50" priority="8" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="45" priority="9" rank="2"/>
+    <cfRule type="top10" dxfId="44" priority="8" bottom="1" rank="1"/>
     <cfRule type="colorScale" priority="7">
       <colorScale>
         <cfvo type="min"/>
@@ -2385,8 +2333,8 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T2:T13">
-    <cfRule type="top10" dxfId="49" priority="6" rank="2"/>
-    <cfRule type="top10" dxfId="48" priority="5" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="43" priority="6" rank="2"/>
+    <cfRule type="top10" dxfId="42" priority="5" bottom="1" rank="1"/>
     <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min"/>
@@ -4877,11 +4825,11 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="top10" dxfId="47" priority="2" bottom="1" rank="1"/>
-    <cfRule type="top10" dxfId="46" priority="3" rank="2"/>
+    <cfRule type="top10" dxfId="41" priority="2" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="40" priority="3" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="P2:P37">
-    <cfRule type="top10" dxfId="45" priority="25" rank="2"/>
+    <cfRule type="top10" dxfId="39" priority="25" rank="2"/>
     <cfRule type="colorScale" priority="19">
       <colorScale>
         <cfvo type="min"/>
@@ -4892,7 +4840,7 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="top10" dxfId="44" priority="24" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="38" priority="24" bottom="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q2:Q37">
     <cfRule type="colorScale" priority="16">
@@ -4905,12 +4853,12 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="top10" dxfId="43" priority="17" bottom="1" rank="1"/>
-    <cfRule type="top10" dxfId="42" priority="18" rank="2"/>
+    <cfRule type="top10" dxfId="37" priority="17" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="36" priority="18" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="R2:R37">
-    <cfRule type="top10" dxfId="41" priority="14" bottom="1" rank="1"/>
-    <cfRule type="top10" dxfId="40" priority="15" rank="2"/>
+    <cfRule type="top10" dxfId="35" priority="14" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="34" priority="15" rank="2"/>
     <cfRule type="colorScale" priority="13">
       <colorScale>
         <cfvo type="min"/>
@@ -4933,12 +4881,12 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="top10" dxfId="39" priority="11" bottom="1" rank="1"/>
-    <cfRule type="top10" dxfId="38" priority="12" rank="2"/>
+    <cfRule type="top10" dxfId="33" priority="11" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="32" priority="12" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="T2:T37">
-    <cfRule type="top10" dxfId="37" priority="9" rank="2"/>
-    <cfRule type="top10" dxfId="36" priority="8" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="31" priority="9" rank="2"/>
+    <cfRule type="top10" dxfId="30" priority="8" bottom="1" rank="1"/>
     <cfRule type="colorScale" priority="7">
       <colorScale>
         <cfvo type="min"/>
@@ -4951,8 +4899,8 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U2:U37">
-    <cfRule type="top10" dxfId="35" priority="6" rank="2"/>
-    <cfRule type="top10" dxfId="34" priority="5" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="29" priority="6" rank="2"/>
+    <cfRule type="top10" dxfId="28" priority="5" bottom="1" rank="1"/>
     <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min"/>
@@ -6663,11 +6611,11 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="top10" dxfId="33" priority="2" bottom="1" rank="1"/>
-    <cfRule type="top10" dxfId="32" priority="3" rank="2"/>
+    <cfRule type="top10" dxfId="27" priority="2" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="26" priority="3" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="P2:P25">
-    <cfRule type="top10" dxfId="31" priority="25" rank="2"/>
+    <cfRule type="top10" dxfId="25" priority="25" rank="2"/>
     <cfRule type="colorScale" priority="19">
       <colorScale>
         <cfvo type="min"/>
@@ -6678,7 +6626,7 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="top10" dxfId="30" priority="24" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="24" priority="24" bottom="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q2:Q25">
     <cfRule type="colorScale" priority="16">
@@ -6691,12 +6639,12 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="top10" dxfId="29" priority="17" bottom="1" rank="1"/>
-    <cfRule type="top10" dxfId="28" priority="18" rank="2"/>
+    <cfRule type="top10" dxfId="23" priority="17" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="22" priority="18" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="R2:R25">
-    <cfRule type="top10" dxfId="27" priority="14" bottom="1" rank="1"/>
-    <cfRule type="top10" dxfId="26" priority="15" rank="2"/>
+    <cfRule type="top10" dxfId="21" priority="14" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="20" priority="15" rank="2"/>
     <cfRule type="colorScale" priority="13">
       <colorScale>
         <cfvo type="min"/>
@@ -6719,12 +6667,12 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="top10" dxfId="25" priority="11" bottom="1" rank="1"/>
-    <cfRule type="top10" dxfId="24" priority="12" rank="2"/>
+    <cfRule type="top10" dxfId="19" priority="11" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="18" priority="12" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="T2:T25">
-    <cfRule type="top10" dxfId="23" priority="9" rank="2"/>
-    <cfRule type="top10" dxfId="22" priority="8" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="17" priority="9" rank="2"/>
+    <cfRule type="top10" dxfId="16" priority="8" bottom="1" rank="1"/>
     <cfRule type="colorScale" priority="7">
       <colorScale>
         <cfvo type="min"/>
@@ -6737,8 +6685,8 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U2:U25">
-    <cfRule type="top10" dxfId="21" priority="6" rank="2"/>
-    <cfRule type="top10" dxfId="20" priority="5" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="15" priority="6" rank="2"/>
+    <cfRule type="top10" dxfId="14" priority="5" bottom="1" rank="1"/>
     <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min"/>
@@ -6759,7 +6707,7 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:U97"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" workbookViewId="0">
+    <sheetView zoomScale="160" workbookViewId="0">
       <selection activeCell="E87" sqref="A87:E87"/>
     </sheetView>
   </sheetViews>
@@ -13087,7 +13035,7 @@
       </filters>
     </filterColumn>
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A63:U97">
-      <sortCondition sortBy="cellColor" ref="A1:A97" dxfId="1"/>
+      <sortCondition sortBy="cellColor" ref="A1:A97" dxfId="56"/>
     </sortState>
   </autoFilter>
   <conditionalFormatting sqref="K2:K97">
@@ -13149,11 +13097,11 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="top10" dxfId="19" priority="2" bottom="1" rank="1"/>
-    <cfRule type="top10" dxfId="18" priority="3" rank="2"/>
+    <cfRule type="top10" dxfId="13" priority="2" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="12" priority="3" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="P2:P97">
-    <cfRule type="top10" dxfId="17" priority="25" rank="2"/>
+    <cfRule type="top10" dxfId="11" priority="25" rank="2"/>
     <cfRule type="colorScale" priority="19">
       <colorScale>
         <cfvo type="min"/>
@@ -13164,7 +13112,7 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="top10" dxfId="16" priority="24" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="10" priority="24" bottom="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q2:Q97">
     <cfRule type="colorScale" priority="16">
@@ -13177,12 +13125,12 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="top10" dxfId="15" priority="17" bottom="1" rank="1"/>
-    <cfRule type="top10" dxfId="14" priority="18" rank="2"/>
+    <cfRule type="top10" dxfId="9" priority="17" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="8" priority="18" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="R2:R97">
-    <cfRule type="top10" dxfId="13" priority="14" bottom="1" rank="1"/>
-    <cfRule type="top10" dxfId="12" priority="15" rank="2"/>
+    <cfRule type="top10" dxfId="7" priority="14" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="6" priority="15" rank="2"/>
     <cfRule type="colorScale" priority="13">
       <colorScale>
         <cfvo type="min"/>
@@ -13205,12 +13153,12 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="top10" dxfId="11" priority="11" bottom="1" rank="1"/>
-    <cfRule type="top10" dxfId="10" priority="12" rank="2"/>
+    <cfRule type="top10" dxfId="5" priority="11" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="4" priority="12" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="T2:T97">
-    <cfRule type="top10" dxfId="9" priority="9" rank="2"/>
-    <cfRule type="top10" dxfId="8" priority="8" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="3" priority="9" rank="2"/>
+    <cfRule type="top10" dxfId="2" priority="8" bottom="1" rank="1"/>
     <cfRule type="colorScale" priority="7">
       <colorScale>
         <cfvo type="min"/>
@@ -13223,8 +13171,8 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U2:U97">
-    <cfRule type="top10" dxfId="7" priority="6" rank="2"/>
-    <cfRule type="top10" dxfId="6" priority="5" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="1" priority="6" rank="2"/>
+    <cfRule type="top10" dxfId="0" priority="5" bottom="1" rank="1"/>
     <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>